<commit_message>
db corrupted error catch
</commit_message>
<xml_diff>
--- a/db_BACKUP_01.xlsx
+++ b/db_BACKUP_01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet sheetId="1" name="Admin" state="visible" r:id="rId4"/>
@@ -19,18 +19,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="518">
   <si>
     <t>allies</t>
   </si>
   <si>
-    <t/>
+    <t>We don't really use this</t>
   </si>
   <si>
     <t>plans</t>
   </si>
   <si>
-    <t>no plans</t>
+    <t>We don't really use this.</t>
   </si>
   <si>
     <t>help</t>
@@ -100,63 +100,33 @@
  - **!notes &lt;tag&gt; create** will add a new alliance to the list that we can add notes for.</t>
   </si>
   <si>
-    <t>finger in the butt</t>
-  </si>
-  <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>169</t>
+    <t>rectum wrecker</t>
   </si>
   <si>
     <t>boricua</t>
   </si>
   <si>
-    <t>171</t>
-  </si>
-  <si>
     <t>bubbarocker</t>
   </si>
   <si>
-    <t>204</t>
-  </si>
-  <si>
     <t>copperpopo</t>
   </si>
   <si>
-    <t>262</t>
-  </si>
-  <si>
     <t>creepingdeath</t>
   </si>
   <si>
-    <t>272</t>
-  </si>
-  <si>
     <t>dirty diapers</t>
   </si>
   <si>
-    <t>285</t>
-  </si>
-  <si>
     <t>dracolatias</t>
   </si>
   <si>
-    <t>268</t>
-  </si>
-  <si>
     <t>i n0mad i</t>
   </si>
   <si>
-    <t>283</t>
-  </si>
-  <si>
     <t>ikandy1</t>
   </si>
   <si>
-    <t>294</t>
-  </si>
-  <si>
     <t>imothe1</t>
   </si>
   <si>
@@ -202,63 +172,51 @@
     <t>xmousecop</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>event</t>
   </si>
   <si>
-    <t>War Reset</t>
-  </si>
-  <si>
-    <t>Final War Reset</t>
-  </si>
-  <si>
     <t>month</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>day</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
     <t>hour</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
     <t>!5min</t>
   </si>
   <si>
-    <t>y</t>
-  </si>
-  <si>
     <t>!1hour</t>
   </si>
   <si>
     <t>!1day</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>SGBR</t>
   </si>
   <si>
     <t>HEALZ</t>
   </si>
   <si>
+    <t>TERRA</t>
+  </si>
+  <si>
     <t>Coolest and most good-looking of all the alliances</t>
   </si>
   <si>
+    <t>also i take back the earlier mean things about healz</t>
+  </si>
+  <si>
+    <t>Fuck Doc Holliday, dude is a certified BITCH</t>
+  </si>
+  <si>
+    <t>Quinn is a good war contact</t>
+  </si>
+  <si>
     <t>Sneak attack often. Spiteful douchebags that will sacrifice resources just to hurt the score of alliances they don't like (us) on principle, even when they have nothing to gain.</t>
   </si>
   <si>
@@ -1456,7 +1414,7 @@
     <t>mjm1976m</t>
   </si>
   <si>
-    <t>05 Oct 2019 21:47:20 GMT</t>
+    <t>29 Oct 2019 23:42:45 GMT</t>
   </si>
   <si>
     <t>117048304646225924</t>
@@ -1465,7 +1423,7 @@
     <t>Boricua</t>
   </si>
   <si>
-    <t>07 Oct 2019 20:15:44 GMT</t>
+    <t>29 Oct 2019 21:52:20 GMT</t>
   </si>
   <si>
     <t>361739579977629697</t>
@@ -1483,25 +1441,19 @@
     <t>621375239909015552</t>
   </si>
   <si>
-    <t>08 Oct 2019 02:23:51 GMT</t>
-  </si>
-  <si>
     <t>621364830418239516</t>
   </si>
   <si>
     <t>pilfer009</t>
   </si>
   <si>
-    <t>08 Oct 2019 03:38:36 GMT</t>
-  </si>
-  <si>
     <t>623316383975079967</t>
   </si>
   <si>
     <t>Draco</t>
   </si>
   <si>
-    <t>08 Oct 2019 01:45:48 GMT</t>
+    <t>15 Oct 2019 15:04:17 GMT</t>
   </si>
   <si>
     <t>484126152571617280</t>
@@ -1510,16 +1462,13 @@
     <t>N0MADIC</t>
   </si>
   <si>
-    <t>08 Oct 2019 02:20:31 GMT</t>
-  </si>
-  <si>
     <t>472627903104811019</t>
   </si>
   <si>
     <t>IKANDY</t>
   </si>
   <si>
-    <t>08 Oct 2019 03:49:17 GMT</t>
+    <t>29 Oct 2019 21:51:20 GMT</t>
   </si>
   <si>
     <t>623622883201253411</t>
@@ -1528,7 +1477,7 @@
     <t>imo the first</t>
   </si>
   <si>
-    <t>07 Oct 2019 20:19:24 GMT</t>
+    <t>12 Oct 2019 03:57:38 GMT</t>
   </si>
   <si>
     <t>463908810373857324</t>
@@ -1537,7 +1486,7 @@
     <t>kash314</t>
   </si>
   <si>
-    <t>07 Oct 2019 23:27:18 GMT</t>
+    <t>15 Oct 2019 19:07:34 GMT</t>
   </si>
   <si>
     <t>395979105700413451</t>
@@ -1546,13 +1495,13 @@
     <t>Korvvish</t>
   </si>
   <si>
-    <t>07 Oct 2019 21:26:09 GMT</t>
+    <t>29 Oct 2019 23:55:25 GMT</t>
   </si>
   <si>
     <t>478053793532084250</t>
   </si>
   <si>
-    <t>03 Oct 2019 00:30:52 GMT</t>
+    <t>15 Oct 2019 06:22:01 GMT</t>
   </si>
   <si>
     <t>409471590988906508</t>
@@ -1561,13 +1510,13 @@
     <t>Nae’blis</t>
   </si>
   <si>
-    <t>08 Oct 2019 10:18:05 GMT</t>
+    <t>29 Oct 2019 23:52:05 GMT</t>
   </si>
   <si>
     <t>453762219042406401</t>
   </si>
   <si>
-    <t>07 Oct 2019 03:03:49 GMT</t>
+    <t>15 Oct 2019 18:16:31 GMT</t>
   </si>
   <si>
     <t>467426493912317953</t>
@@ -1576,7 +1525,7 @@
     <t>PapaMarsh</t>
   </si>
   <si>
-    <t>11 Oct 2019 19:59:58 GMT</t>
+    <t>29 Oct 2019 23:59:03 GMT</t>
   </si>
   <si>
     <t>214042704357621760</t>
@@ -1585,7 +1534,7 @@
     <t>dancingpotato</t>
   </si>
   <si>
-    <t>07 Oct 2019 15:59:45 GMT</t>
+    <t>15 Oct 2019 15:28:39 GMT</t>
   </si>
   <si>
     <t>370999241688219690</t>
@@ -1600,7 +1549,7 @@
     <t>Ricky</t>
   </si>
   <si>
-    <t>08 Oct 2019 02:08:50 GMT</t>
+    <t>15 Oct 2019 01:01:59 GMT</t>
   </si>
   <si>
     <t>621404757042659328</t>
@@ -1615,7 +1564,7 @@
     <t>SarcasticAhole</t>
   </si>
   <si>
-    <t>08 Oct 2019 08:25:18 GMT</t>
+    <t>29 Oct 2019 23:53:45 GMT</t>
   </si>
   <si>
     <t>305697563175157760</t>
@@ -1624,19 +1573,13 @@
     <t>shooty-pants</t>
   </si>
   <si>
-    <t>428221019409350666</t>
-  </si>
-  <si>
-    <t>TeamGB</t>
-  </si>
-  <si>
     <t>246021971601522688</t>
   </si>
   <si>
     <t>SilviuPOWER</t>
   </si>
   <si>
-    <t>08 Oct 2019 10:23:26 GMT</t>
+    <t>15 Oct 2019 19:33:56 GMT</t>
   </si>
   <si>
     <t>420761034941530113</t>
@@ -1645,13 +1588,7 @@
     <t>mousecop</t>
   </si>
   <si>
-    <t>08 Oct 2019 03:59:17 GMT</t>
-  </si>
-  <si>
-    <t>262441739523063809</t>
-  </si>
-  <si>
-    <t>jimmylalao</t>
+    <t>13 Oct 2019 01:50:43 GMT</t>
   </si>
   <si>
     <t>431633842634358794</t>
@@ -1667,6 +1604,12 @@
   </si>
   <si>
     <t>PapaBot</t>
+  </si>
+  <si>
+    <t>482657328320217139</t>
+  </si>
+  <si>
+    <t>ballndp</t>
   </si>
 </sst>
 </file>
@@ -2117,215 +2060,137 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2335,7 +2200,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="B1" sqref="B1"/>
@@ -2343,102 +2208,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2448,7 +2250,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="B10" sqref="B10"/>
@@ -2456,25 +2258,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>68</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2497,1837 +2315,1837 @@
   <sheetData>
     <row r="1" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
     </row>
     <row r="46" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
     </row>
     <row r="51" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="53" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
     </row>
     <row r="57" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
     </row>
     <row r="58" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
     </row>
     <row r="59" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
     </row>
     <row r="63" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
     </row>
     <row r="66" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
     </row>
     <row r="67" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
     </row>
     <row r="68" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
     </row>
     <row r="69" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
     </row>
     <row r="70" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="71" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
     </row>
     <row r="72" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
     </row>
     <row r="73" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
     </row>
     <row r="74" ht="15" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
     </row>
     <row r="75" ht="15" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
     </row>
     <row r="76" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
     </row>
     <row r="77" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
     </row>
     <row r="79" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
     </row>
     <row r="80" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
     </row>
     <row r="82" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
     </row>
     <row r="83" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="85" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
     </row>
     <row r="86" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
     </row>
     <row r="88" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
     </row>
     <row r="89" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
     </row>
     <row r="91" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
     </row>
     <row r="92" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
     </row>
     <row r="94" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
     </row>
     <row r="95" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
     </row>
     <row r="97" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
     </row>
     <row r="98" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
     </row>
     <row r="100" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
     </row>
     <row r="101" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
     </row>
     <row r="103" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
     </row>
     <row r="104" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="106" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="107" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
     </row>
     <row r="109" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
     </row>
     <row r="110" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
     </row>
     <row r="112" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
     </row>
     <row r="113" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
     </row>
     <row r="115" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
     </row>
     <row r="116" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
     </row>
     <row r="118" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
     </row>
     <row r="119" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
     </row>
     <row r="121" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
     </row>
     <row r="122" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
     </row>
     <row r="124" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
     </row>
     <row r="125" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
     </row>
     <row r="127" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
     </row>
     <row r="128" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
     </row>
     <row r="130" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
     </row>
     <row r="131" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
     </row>
     <row r="133" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
     </row>
     <row r="134" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
     </row>
     <row r="136" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
     </row>
     <row r="137" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
     </row>
     <row r="139" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
     </row>
     <row r="140" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
     </row>
     <row r="142" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
     </row>
     <row r="143" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
     </row>
     <row r="145" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
     </row>
     <row r="146" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
     </row>
     <row r="148" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
     </row>
     <row r="149" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
     </row>
     <row r="151" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
     </row>
     <row r="152" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
     </row>
     <row r="154" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
     </row>
     <row r="155" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
     </row>
     <row r="157" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
     </row>
     <row r="158" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
     </row>
     <row r="160" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
     </row>
     <row r="161" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
     </row>
     <row r="163" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
     </row>
     <row r="164" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
     </row>
     <row r="166" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
     </row>
     <row r="167" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
     </row>
     <row r="169" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
     </row>
     <row r="170" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="172" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
     </row>
     <row r="173" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
     </row>
     <row r="175" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
     </row>
     <row r="176" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
     </row>
     <row r="178" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
     </row>
     <row r="179" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="181" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
     </row>
     <row r="182" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
     </row>
     <row r="184" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
     </row>
     <row r="185" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
     </row>
     <row r="187" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
     </row>
     <row r="188" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
     </row>
     <row r="190" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
     </row>
     <row r="191" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
     </row>
     <row r="193" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
     </row>
     <row r="194" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
     </row>
     <row r="196" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
     </row>
     <row r="197" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
     </row>
     <row r="199" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
     </row>
     <row r="200" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
     </row>
     <row r="202" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
     </row>
     <row r="203" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
     </row>
     <row r="205" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
     </row>
     <row r="206" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
     </row>
     <row r="208" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
     </row>
     <row r="209" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="211" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
     </row>
     <row r="212" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
     </row>
     <row r="214" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
     </row>
     <row r="215" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
     </row>
     <row r="217" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
     </row>
     <row r="218" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
     </row>
     <row r="220" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="221" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="223" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
     </row>
     <row r="224" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
     </row>
     <row r="226" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
     </row>
     <row r="227" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
     </row>
     <row r="229" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
     </row>
     <row r="230" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
     </row>
     <row r="232" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
     </row>
     <row r="233" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
     </row>
     <row r="235" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
     </row>
     <row r="236" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
     </row>
     <row r="238" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
     </row>
     <row r="239" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
     </row>
     <row r="241" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
     </row>
     <row r="242" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
     </row>
     <row r="244" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
     </row>
     <row r="245" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
     </row>
     <row r="247" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
     </row>
     <row r="248" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
     </row>
     <row r="250" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
     </row>
     <row r="251" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
     </row>
     <row r="253" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
     </row>
     <row r="254" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
     </row>
     <row r="256" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
     </row>
     <row r="257" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="259" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
     </row>
     <row r="260" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
     </row>
     <row r="262" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
     </row>
     <row r="263" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
     </row>
     <row r="265" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
     </row>
     <row r="266" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
     </row>
     <row r="268" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
     </row>
     <row r="269" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
     </row>
     <row r="271" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
     </row>
     <row r="272" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
     </row>
     <row r="274" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
     </row>
     <row r="275" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
     </row>
     <row r="277" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
     </row>
     <row r="278" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
     </row>
     <row r="280" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
     </row>
     <row r="281" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
     </row>
     <row r="283" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
     </row>
     <row r="284" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
     </row>
     <row r="286" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
     </row>
     <row r="287" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
     </row>
     <row r="289" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
     </row>
     <row r="290" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
     </row>
     <row r="292" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
     </row>
     <row r="293" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
     </row>
     <row r="295" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
     </row>
     <row r="296" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
     </row>
     <row r="298" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
     </row>
     <row r="299" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
     </row>
     <row r="301" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
     </row>
     <row r="302" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
     </row>
     <row r="304" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
     </row>
     <row r="305" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
     </row>
     <row r="307" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
     </row>
     <row r="308" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="310" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
-        <v>370</v>
+        <v>356</v>
       </c>
     </row>
     <row r="311" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
     </row>
     <row r="313" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
     </row>
     <row r="314" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
     </row>
     <row r="316" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
     </row>
     <row r="317" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
     </row>
     <row r="319" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
-        <v>376</v>
+        <v>362</v>
       </c>
     </row>
     <row r="320" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
-        <v>377</v>
+        <v>363</v>
       </c>
     </row>
     <row r="322" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
     </row>
     <row r="323" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
     </row>
     <row r="325" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
     </row>
     <row r="326" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
     </row>
     <row r="328" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
-        <v>382</v>
+        <v>368</v>
       </c>
     </row>
     <row r="329" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
     </row>
     <row r="331" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
     </row>
     <row r="332" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
     </row>
     <row r="334" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
     </row>
     <row r="335" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
     </row>
     <row r="337" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
-        <v>388</v>
+        <v>374</v>
       </c>
     </row>
     <row r="338" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
     </row>
     <row r="340" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
-        <v>390</v>
+        <v>376</v>
       </c>
     </row>
     <row r="341" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
     </row>
     <row r="343" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
     </row>
     <row r="344" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
-        <v>393</v>
+        <v>379</v>
       </c>
     </row>
     <row r="346" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
     </row>
     <row r="347" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
     </row>
     <row r="349" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
     </row>
     <row r="350" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
     </row>
     <row r="352" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
     </row>
     <row r="353" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
     </row>
     <row r="355" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
     </row>
     <row r="356" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
     </row>
     <row r="358" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
     </row>
     <row r="359" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
     </row>
     <row r="361" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
     </row>
     <row r="362" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
     </row>
     <row r="364" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
     </row>
     <row r="365" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
     </row>
     <row r="367" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
     </row>
     <row r="368" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
     </row>
     <row r="370" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
     </row>
     <row r="371" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
     </row>
     <row r="373" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
     </row>
     <row r="374" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
     </row>
     <row r="376" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
     </row>
     <row r="377" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
     </row>
     <row r="379" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="380" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="382" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
     </row>
     <row r="383" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
     </row>
     <row r="385" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" s="1" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
     </row>
     <row r="386" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
     </row>
     <row r="388" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
     </row>
     <row r="389" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
     </row>
     <row r="391" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
     </row>
     <row r="392" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
     </row>
     <row r="394" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
     </row>
     <row r="395" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
-        <v>427</v>
+        <v>413</v>
       </c>
     </row>
     <row r="397" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
-        <v>428</v>
+        <v>414</v>
       </c>
     </row>
     <row r="398" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
-        <v>429</v>
+        <v>415</v>
       </c>
     </row>
     <row r="400" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
-        <v>430</v>
+        <v>416</v>
       </c>
     </row>
     <row r="401" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
-        <v>431</v>
+        <v>417</v>
       </c>
     </row>
     <row r="403" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
     </row>
     <row r="404" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
     </row>
     <row r="406" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
-        <v>434</v>
+        <v>420</v>
       </c>
     </row>
     <row r="407" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
-        <v>435</v>
+        <v>421</v>
       </c>
     </row>
     <row r="409" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A409" s="1" t="s">
-        <v>436</v>
+        <v>422</v>
       </c>
     </row>
     <row r="410" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A410" s="1" t="s">
-        <v>437</v>
+        <v>423</v>
       </c>
     </row>
     <row r="412" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
     </row>
     <row r="413" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
     </row>
     <row r="415" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A415" s="1" t="s">
-        <v>440</v>
+        <v>426</v>
       </c>
     </row>
     <row r="416" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A416" s="1" t="s">
-        <v>441</v>
+        <v>427</v>
       </c>
     </row>
     <row r="418" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A418" s="1" t="s">
-        <v>442</v>
+        <v>428</v>
       </c>
     </row>
     <row r="419" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A419" s="1" t="s">
-        <v>443</v>
+        <v>429</v>
       </c>
     </row>
     <row r="421" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A421" s="1" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
     </row>
     <row r="422" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A422" s="1" t="s">
-        <v>445</v>
+        <v>431</v>
       </c>
     </row>
     <row r="424" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A424" s="1" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
     </row>
     <row r="425" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A425" s="1" t="s">
-        <v>447</v>
+        <v>433</v>
       </c>
     </row>
     <row r="427" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A427" s="1" t="s">
-        <v>448</v>
+        <v>434</v>
       </c>
     </row>
     <row r="428" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A428" s="1" t="s">
-        <v>449</v>
+        <v>435</v>
       </c>
     </row>
     <row r="430" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A430" s="1" t="s">
-        <v>450</v>
+        <v>436</v>
       </c>
     </row>
     <row r="431" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A431" s="1" t="s">
-        <v>451</v>
+        <v>437</v>
       </c>
     </row>
     <row r="433" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A433" s="1" t="s">
-        <v>452</v>
+        <v>438</v>
       </c>
     </row>
     <row r="434" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A434" s="1" t="s">
-        <v>453</v>
+        <v>439</v>
       </c>
     </row>
     <row r="436" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A436" s="1" t="s">
-        <v>454</v>
+        <v>440</v>
       </c>
     </row>
     <row r="437" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A437" s="1" t="s">
-        <v>455</v>
+        <v>441</v>
       </c>
     </row>
     <row r="439" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A439" s="1" t="s">
-        <v>456</v>
+        <v>442</v>
       </c>
     </row>
     <row r="440" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A440" s="1" t="s">
-        <v>457</v>
+        <v>443</v>
       </c>
     </row>
     <row r="442" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A442" s="1" t="s">
-        <v>458</v>
+        <v>444</v>
       </c>
     </row>
     <row r="443" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A443" s="1" t="s">
-        <v>459</v>
+        <v>445</v>
       </c>
     </row>
     <row r="445" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A445" s="1" t="s">
-        <v>460</v>
+        <v>446</v>
       </c>
     </row>
     <row r="446" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A446" s="1" t="s">
-        <v>461</v>
+        <v>447</v>
       </c>
     </row>
     <row r="448" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A448" s="1" t="s">
-        <v>462</v>
+        <v>448</v>
       </c>
     </row>
     <row r="449" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A449" s="1" t="s">
-        <v>463</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -4337,302 +4155,294 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>464</v>
+        <v>450</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>465</v>
+        <v>451</v>
       </c>
       <c r="C1" t="s">
-        <v>466</v>
+        <v>452</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>467</v>
+        <v>453</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>468</v>
+        <v>454</v>
       </c>
       <c r="C2" t="s">
-        <v>469</v>
+        <v>455</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>470</v>
+        <v>456</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>471</v>
+        <v>457</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>472</v>
+        <v>458</v>
       </c>
       <c r="C4" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>474</v>
+        <v>460</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>475</v>
+        <v>455</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>476</v>
+        <v>461</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>477</v>
+        <v>462</v>
       </c>
       <c r="C6" t="s">
-        <v>478</v>
+        <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>479</v>
+        <v>463</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>480</v>
+        <v>464</v>
       </c>
       <c r="C7" t="s">
-        <v>481</v>
+        <v>465</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>482</v>
+        <v>466</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>483</v>
+        <v>467</v>
       </c>
       <c r="C8" t="s">
-        <v>484</v>
+        <v>455</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>485</v>
+        <v>468</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>486</v>
+        <v>469</v>
       </c>
       <c r="C9" t="s">
-        <v>487</v>
+        <v>470</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>488</v>
+        <v>471</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>489</v>
+        <v>472</v>
       </c>
       <c r="C10" t="s">
-        <v>490</v>
+        <v>473</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>491</v>
+        <v>474</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>492</v>
+        <v>475</v>
       </c>
       <c r="C11" t="s">
-        <v>493</v>
+        <v>476</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>494</v>
+        <v>477</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>495</v>
+        <v>478</v>
       </c>
       <c r="C12" t="s">
-        <v>496</v>
+        <v>479</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>497</v>
+        <v>480</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>498</v>
+        <v>481</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>499</v>
+        <v>482</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>500</v>
+        <v>483</v>
       </c>
       <c r="C14" t="s">
-        <v>501</v>
+        <v>484</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>502</v>
+        <v>485</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>503</v>
+        <v>486</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>504</v>
+        <v>487</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>505</v>
+        <v>488</v>
       </c>
       <c r="C16" t="s">
-        <v>506</v>
+        <v>489</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>507</v>
+        <v>490</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>508</v>
+        <v>491</v>
       </c>
       <c r="C17" t="s">
-        <v>509</v>
+        <v>492</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>510</v>
+        <v>493</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>511</v>
+        <v>494</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>512</v>
+        <v>495</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>513</v>
+        <v>496</v>
       </c>
       <c r="C19" t="s">
-        <v>514</v>
+        <v>497</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>515</v>
+        <v>498</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>516</v>
+        <v>499</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>517</v>
+        <v>500</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>518</v>
+        <v>501</v>
       </c>
       <c r="C21" t="s">
-        <v>519</v>
+        <v>502</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>520</v>
+        <v>503</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>522</v>
+        <v>505</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>523</v>
+        <v>506</v>
+      </c>
+      <c r="C23" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>524</v>
+        <v>508</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>525</v>
+        <v>509</v>
       </c>
       <c r="C24" t="s">
-        <v>526</v>
+        <v>510</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>527</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>528</v>
+      <c r="A25" t="s">
+        <v>511</v>
+      </c>
+      <c r="B25" t="s">
+        <v>512</v>
       </c>
       <c r="C25" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>530</v>
+        <v>514</v>
       </c>
       <c r="B26" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>515</v>
+      </c>
+      <c r="C26" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>532</v>
+        <v>516</v>
       </c>
       <c r="B27" t="s">
-        <v>533</v>
-      </c>
-      <c r="C27" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>535</v>
-      </c>
-      <c r="B28" t="s">
-        <v>536</v>
-      </c>
-      <c r="C28" t="s">
-        <v>506</v>
+        <v>517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
console fix & db
</commit_message>
<xml_diff>
--- a/db_BACKUP_01.xlsx
+++ b/db_BACKUP_01.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="435">
   <si>
     <t>Welcome Message</t>
   </si>
@@ -77,7 +77,7 @@
     <t>Papa Marsh; Mini Marsh; Donatello</t>
   </si>
   <si>
-    <t>4/16 at 23:18</t>
+    <t>4/17 at 13:59</t>
   </si>
   <si>
     <t>522247064315494420</t>
@@ -98,9 +98,6 @@
     <t>PapaBot</t>
   </si>
   <si>
-    <t>4/17 at 8:59</t>
-  </si>
-  <si>
     <t>700391520041173113</t>
   </si>
   <si>
@@ -120,6 +117,12 @@
   </si>
   <si>
     <t>4/16 at 22:23</t>
+  </si>
+  <si>
+    <t>406129972982317068</t>
+  </si>
+  <si>
+    <t>Sidekick II</t>
   </si>
   <si>
     <t>event</t>
@@ -1704,1837 +1707,1837 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A301" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A302" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A304" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A310" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A311" s="2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A316" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A317" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A319" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A320" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A322" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A323" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A328" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A329" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A331" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A332" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A334" s="2" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A335" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A340" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A341" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A343" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A347" s="2" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A350" s="2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A352" s="2" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A353" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" s="2" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A356" s="2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" s="2" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A359" s="2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A361" s="2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A362" s="2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364" s="2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A368" s="2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A370" s="2" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A371" s="2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A379" s="2" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A380" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" s="2" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" s="2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A386" s="2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A391" s="2" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A392" s="2" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A394" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A395" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398" s="2" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A400" s="2" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A401" s="2" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A403" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A404" s="2" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A406" s="2" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A407" s="2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A409" s="2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A410" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A412" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A413" s="2" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A415" s="2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A416" s="2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A418" s="2" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A419" s="2" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A421" s="2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A422" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A424" s="2" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A425" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A427" s="2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A428" s="2" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A430" s="2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A431" s="2" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A433" s="2" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A434" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A436" s="2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A437" s="2" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A439" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A440" s="2" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A442" s="2" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A443" s="2" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A445" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A446" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A448" s="2" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A449" s="2" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -3554,37 +3557,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -3594,7 +3597,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="C2" sqref="C2"/>
@@ -3680,32 +3683,43 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>27</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>